<commit_message>
Modded some xlsx formatting...
</commit_message>
<xml_diff>
--- a/Server/WorkOrderExcelLogs/666.xlsx
+++ b/Server/WorkOrderExcelLogs/666.xlsx
@@ -10,6 +10,7 @@
     <s:sheet name="Work Order Sumary" sheetId="1" r:id="rId1"/>
     <s:sheet name="Run#1" sheetId="2" r:id="rId2"/>
     <s:sheet name="Run#11" sheetId="3" r:id="rId3"/>
+    <s:sheet name="Run#2" sheetId="4" r:id="rId4"/>
   </s:sheets>
   <s:definedNames/>
   <s:calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
@@ -17,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="41">
   <si>
     <t>(04/09/14) @ 21:17:31</t>
   </si>
@@ -25,6 +26,9 @@
     <t>(04/09/14) @ 21:17:44</t>
   </si>
   <si>
+    <t>(04/09/14) @ 21:42:19</t>
+  </si>
+  <si>
     <t>(322, Total, 100, 21:17:53)</t>
   </si>
   <si>
@@ -49,10 +53,19 @@
     <t xml:space="preserve">666:  (21:17:58,21:18:29) </t>
   </si>
   <si>
+    <t xml:space="preserve">666:  (21:17:58,21:42:23) </t>
+  </si>
+  <si>
     <t xml:space="preserve">66:  (21:18:27,21:18:29) </t>
   </si>
   <si>
+    <t xml:space="preserve">66:  (21:18:27,21:42:23) </t>
+  </si>
+  <si>
     <t xml:space="preserve">858:  (21:18:03,21:18:29) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">858:  (21:18:03,21:42:23) </t>
   </si>
   <si>
     <t xml:space="preserve">Box Count: </t>
@@ -463,7 +476,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,7 +494,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B1" t="n">
         <v>666</v>
@@ -489,42 +502,42 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -535,7 +548,7 @@
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
@@ -555,7 +568,7 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D6" t="n">
         <v>100</v>
@@ -564,6 +577,26 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -590,7 +623,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B1" t="n">
         <v>11</v>
@@ -598,7 +631,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -606,15 +639,15 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B4" t="n">
         <v>0</v>
@@ -622,15 +655,15 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B6" t="n">
         <v>0</v>
@@ -638,15 +671,15 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B8" t="n">
         <v>0</v>
@@ -654,60 +687,60 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -719,7 +752,170 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="9.1"/>
+    <col customWidth="1" max="2" min="2" width="9.1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -733,7 +929,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B1" t="n">
         <v>11</v>
@@ -741,39 +937,39 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B4" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B6" t="n">
         <v>0</v>
@@ -781,15 +977,15 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B8" t="n">
         <v>0</v>
@@ -797,80 +993,75 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
-        <v>2</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
-      <c r="A28" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" t="s">
-        <v>31</v>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>